<commit_message>
Deploying to gh-pages from @ eurovibes/com4bbb@82d1824c6370e45de1223c278c0f35fdd320c161 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/com4bbb-bom_0.1.xlsx
+++ b/Fabrication/BoM/com4bbb-bom_0.1.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="85">
   <si>
     <t>Row</t>
   </si>
@@ -104,126 +104,114 @@
     <t>Conn_01x02</t>
   </si>
   <si>
-    <t>RS485</t>
-  </si>
-  <si>
-    <t>TerminalBlock_WAGO_236-102_1x02_P5.00mm_45Degree</t>
+    <t>PWR</t>
+  </si>
+  <si>
+    <t>TerminalBlock_Phoenix_MPT-0,5-2-2.54_1x02_P2.54mm_Horizontal</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>JP105 JP106 JP107 JP108</t>
-  </si>
-  <si>
-    <t>Jumper_NO_Small</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>SolderJumper-2_P1.3mm_Open_RoundedPad1.0x1.5mm</t>
+    <t>JP101 JP102 JP103 JP104</t>
+  </si>
+  <si>
+    <t>Jumper_3_Open</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>SolderJumper-3_P1.3mm_Open_RoundedPad1.0x1.5mm</t>
   </si>
   <si>
     <t>6</t>
   </si>
   <si>
-    <t>JP101 JP102 JP103 JP104</t>
-  </si>
-  <si>
-    <t>Jumper_3_Open</t>
-  </si>
-  <si>
-    <t>TX</t>
-  </si>
-  <si>
-    <t>SolderJumper-3_P1.3mm_Open_RoundedPad1.0x1.5mm</t>
+    <t>P8 P9</t>
+  </si>
+  <si>
+    <t>Conn_02x23_Odd_Even</t>
+  </si>
+  <si>
+    <t>BeagleBone_Black_Header</t>
+  </si>
+  <si>
+    <t>PinHeader_2x23_P2.54mm_Vertical</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
-    <t>P8 P9</t>
-  </si>
-  <si>
-    <t>Conn_02x23_Odd_Even</t>
-  </si>
-  <si>
-    <t>BeagleBone_Black_Header</t>
-  </si>
-  <si>
-    <t>Socket_BeagleBone_Black</t>
+    <t>R101 R102 R103 R104 R105 R106 R107 R108 R109 R110 R111 R112 R113 R114 R115 R116 R117</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>1 kΩ</t>
+  </si>
+  <si>
+    <t>R_0402_1005Metric</t>
+  </si>
+  <si>
+    <t>17</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
-    <t>R101 R102 R103 R104 R105 R106 R107 R108 R109 R110 R111 R112 R113 R114 R115 R116 R117</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>1 kΩ</t>
-  </si>
-  <si>
-    <t>R_0402_1005Metric</t>
-  </si>
-  <si>
-    <t>17</t>
+    <t>SW101 SW102</t>
+  </si>
+  <si>
+    <t>SW_Push_45deg</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>SW_PUSH_6mm</t>
   </si>
   <si>
     <t>9</t>
   </si>
   <si>
-    <t>SW101 SW102</t>
-  </si>
-  <si>
-    <t>SW_Push_45deg</t>
-  </si>
-  <si>
-    <t>Reset</t>
-  </si>
-  <si>
-    <t>SW_PUSH_6mm</t>
+    <t>U102</t>
+  </si>
+  <si>
+    <t>AT24CS64-SSHM</t>
+  </si>
+  <si>
+    <t>AT24C512C-SSHD-T</t>
+  </si>
+  <si>
+    <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
   </si>
   <si>
     <t>10</t>
   </si>
   <si>
+    <t>U104</t>
+  </si>
+  <si>
+    <t>ESP32-WROOM-32U</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>U103</t>
   </si>
   <si>
-    <t>AT24CS64-SSHM</t>
-  </si>
-  <si>
-    <t>AT24C512C-SSHD-T</t>
-  </si>
-  <si>
-    <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>11</t>
+    <t>SP3485EN</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
   <si>
     <t>U101</t>
   </si>
   <si>
-    <t>ESP32-WROOM-32U</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>U102</t>
-  </si>
-  <si>
-    <t>SP3485EN</t>
-  </si>
-  <si>
-    <t>U104</t>
-  </si>
-  <si>
     <t>WPMDH1100xx1S</t>
   </si>
   <si>
@@ -257,7 +245,7 @@
     <t>KiCad Version:</t>
   </si>
   <si>
-    <t>5.1.9+dfsg1-1~bpo10+1</t>
+    <t>9.0.1+1</t>
   </si>
   <si>
     <t>Component Groups:</t>
@@ -273,6 +261,9 @@
   </si>
   <si>
     <t>Total Components:</t>
+  </si>
+  <si>
+    <t>Columns colors</t>
   </si>
   <si>
     <t>KiCad Fields (default)</t>
@@ -385,34 +376,34 @@
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="justify" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="justify" wrapText="1"/>
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="justify" wrapText="1"/>
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="justify" wrapText="1"/>
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="justify" wrapText="1"/>
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="justify" wrapText="1"/>
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="justify" wrapText="1"/>
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="justify" wrapText="1"/>
+      <alignment horizontal="centerContinuous" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -425,7 +416,7 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -440,7 +431,16 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="logo.png"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+            <a:ext uri="{C183D7F6-B498-43B3-948B-1728B52AA6E4}">
+              <adec:decorative xmlns:adec="http://schemas.microsoft.com/office/drawing/2017/decorative" val="1"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -751,7 +751,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -767,14 +767,14 @@
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
     <col min="7" max="7" width="23.7109375" customWidth="1"/>
-    <col min="8" max="8" width="53.7109375" customWidth="1"/>
+    <col min="8" max="8" width="60.7109375" customWidth="1"/>
     <col min="9" max="9" width="21.7109375" customWidth="1"/>
     <col min="10" max="10" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -786,55 +786,55 @@
     </row>
     <row r="2" spans="1:10">
       <c r="C2" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F2" s="3">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="C3" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F3" s="3">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F4" s="3">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="C5" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -842,16 +842,16 @@
     </row>
     <row r="6" spans="1:10">
       <c r="C6" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F6" s="3">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -950,7 +950,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30.0" customHeight="1">
+    <row r="11" spans="1:10" ht="30" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
@@ -1075,10 +1075,10 @@
         <v>14</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="30" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>40</v>
       </c>
@@ -1107,39 +1107,39 @@
         <v>14</v>
       </c>
       <c r="J15" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" s="8" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="30.0" customHeight="1">
-      <c r="A16" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1171,7 +1171,7 @@
         <v>14</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1185,7 +1185,7 @@
         <v>58</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>14</v>
@@ -1197,7 +1197,7 @@
         <v>14</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I18" s="10" t="s">
         <v>14</v>
@@ -1208,16 +1208,16 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>63</v>
-      </c>
       <c r="D19" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>14</v>
@@ -1229,7 +1229,7 @@
         <v>14</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="I19" s="7" t="s">
         <v>14</v>
@@ -1240,16 +1240,16 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>66</v>
-      </c>
       <c r="D20" s="9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>14</v>
@@ -1261,44 +1261,12 @@
         <v>14</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>14</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J21" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1319,38 +1287,42 @@
     <hyperlink ref="G18" r:id="rId10"/>
     <hyperlink ref="G19" r:id="rId11"/>
     <hyperlink ref="G20" r:id="rId12"/>
-    <hyperlink ref="G21" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId14"/>
+  <drawing r:id="rId13"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="6" t="s">
-        <v>85</v>
+      <c r="A1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="5" t="s">
-        <v>86</v>
+      <c r="A2" s="6" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="7" t="s">
-        <v>87</v>
+      <c r="A3" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ eurovibes/com4bbb@703e94b3b70e2b39cedc4a1287db2450ea9a1f9e 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/com4bbb-bom_0.1.xlsx
+++ b/Fabrication/BoM/com4bbb-bom_0.1.xlsx
@@ -18,33 +18,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="104">
   <si>
     <t>Row</t>
   </si>
   <si>
-    <t>Referencias</t>
-  </si>
-  <si>
-    <t>Parte</t>
-  </si>
-  <si>
-    <t>Valor</t>
+    <t>References</t>
+  </si>
+  <si>
+    <t>Part</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
   <si>
     <t>P/N</t>
   </si>
   <si>
-    <t>Fabricante</t>
-  </si>
-  <si>
-    <t>Cod. Digi-Key</t>
+    <t>Manufacture</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Supplier P/N</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
   <si>
     <t>Footprint</t>
   </si>
   <si>
-    <t>Descripción</t>
+    <t>Description</t>
   </si>
   <si>
     <t>Quantity Per PCB</t>
@@ -65,9 +71,15 @@
     <t/>
   </si>
   <si>
+    <t>Samsung Electro-Mechanics</t>
+  </si>
+  <si>
     <t>C_0402_1005Metric</t>
   </si>
   <si>
+    <t>Unpolarized capacitor</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
@@ -80,6 +92,9 @@
     <t>D_DO-41_SOD81_P10.16mm_Horizontal</t>
   </si>
   <si>
+    <t>400V 1A General Purpose Rectifier Diode, DO-41</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
@@ -89,9 +104,15 @@
     <t>LED</t>
   </si>
   <si>
+    <t>Hubei KENTO Elec</t>
+  </si>
+  <si>
     <t>LED_0603_1608Metric</t>
   </si>
   <si>
+    <t>Light emitting diode</t>
+  </si>
+  <si>
     <t>13</t>
   </si>
   <si>
@@ -110,6 +131,9 @@
     <t>TerminalBlock_Phoenix_MPT-0,5-2-2.54_1x02_P2.54mm_Horizontal</t>
   </si>
   <si>
+    <t>Generic connector, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
     <t>5</t>
   </si>
   <si>
@@ -125,6 +149,9 @@
     <t>SolderJumper-3_P1.3mm_Open_RoundedPad1.0x1.5mm</t>
   </si>
   <si>
+    <t>Jumper, 3-pole, both open</t>
+  </si>
+  <si>
     <t>6</t>
   </si>
   <si>
@@ -140,6 +167,9 @@
     <t>PinHeader_2x23_P2.54mm_Vertical</t>
   </si>
   <si>
+    <t>Generic connector, double row, 02x23, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
     <t>7</t>
   </si>
   <si>
@@ -152,9 +182,15 @@
     <t>1 kΩ</t>
   </si>
   <si>
+    <t>UNI-ROYAL(Uniroyal Elec)</t>
+  </si>
+  <si>
     <t>R_0402_1005Metric</t>
   </si>
   <si>
+    <t>Resistor</t>
+  </si>
+  <si>
     <t>17</t>
   </si>
   <si>
@@ -173,6 +209,9 @@
     <t>SW_PUSH_6mm</t>
   </si>
   <si>
+    <t>Push button switch, normally open, two pins, 45° tilted</t>
+  </si>
+  <si>
     <t>9</t>
   </si>
   <si>
@@ -185,9 +224,15 @@
     <t>AT24C512C-SSHD-T</t>
   </si>
   <si>
+    <t>Microchip Tech</t>
+  </si>
+  <si>
     <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
   </si>
   <si>
+    <t>I2C Serial EEPROM, 64Kb (8192x8) with Unique Serial Number, SO8</t>
+  </si>
+  <si>
     <t>10</t>
   </si>
   <si>
@@ -197,6 +242,12 @@
     <t>ESP32-WROOM-32U</t>
   </si>
   <si>
+    <t>Espressif Systems</t>
+  </si>
+  <si>
+    <t>RF Module, ESP32-D0WD SoC, Wi-Fi 802.11b/g/n, Bluetooth, BLE, 32-bit, 2.7-3.6V, external antenna, SMD</t>
+  </si>
+  <si>
     <t>11</t>
   </si>
   <si>
@@ -204,6 +255,12 @@
   </si>
   <si>
     <t>SP3485EN</t>
+  </si>
+  <si>
+    <t>MaxLinear</t>
+  </si>
+  <si>
+    <t>Industrial 3.3V Low Power Half-Duplex RS-485 Transceiver 10Mbps, SOIC-8</t>
   </si>
   <si>
     <t>12</t>
@@ -751,7 +808,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -765,16 +822,18 @@
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="28.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" customWidth="1"/>
-    <col min="8" max="8" width="60.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" customWidth="1"/>
-    <col min="10" max="10" width="26.7109375" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="60.7109375" customWidth="1"/>
+    <col min="11" max="11" width="60.7109375" customWidth="1"/>
+    <col min="12" max="12" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="32" customHeight="1">
+    <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -783,78 +842,80 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="F2" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="F3" s="3">
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="F4" s="3">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="F6" s="3">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:12">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -885,408 +946,486 @@
       <c r="J8" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="8" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="30" customHeight="1">
+        <v>16</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" customHeight="1">
       <c r="A11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30" customHeight="1">
+      <c r="A12" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="L12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="L13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+    </row>
+    <row r="14" spans="1:12" ht="45" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>39</v>
+        <v>16</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="30" customHeight="1">
+        <v>16</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>44</v>
+        <v>16</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>16</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="8" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>50</v>
+        <v>16</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+        <v>16</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="30" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>55</v>
+        <v>16</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+        <v>16</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>58</v>
+        <v>16</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <v>16</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>14</v>
+        <v>79</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>55</v>
+        <v>16</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+        <v>16</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="8" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>64</v>
+        <v>16</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>10</v>
+        <v>16</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="C1:L1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G9" r:id="rId1"/>
-    <hyperlink ref="G10" r:id="rId2"/>
-    <hyperlink ref="G11" r:id="rId3"/>
-    <hyperlink ref="G12" r:id="rId4"/>
-    <hyperlink ref="G13" r:id="rId5"/>
-    <hyperlink ref="G14" r:id="rId6"/>
-    <hyperlink ref="G15" r:id="rId7"/>
-    <hyperlink ref="G16" r:id="rId8"/>
-    <hyperlink ref="G17" r:id="rId9"/>
-    <hyperlink ref="G18" r:id="rId10"/>
-    <hyperlink ref="G19" r:id="rId11"/>
-    <hyperlink ref="G20" r:id="rId12"/>
+    <hyperlink ref="H9" r:id="rId1"/>
+    <hyperlink ref="H10" r:id="rId2"/>
+    <hyperlink ref="H11" r:id="rId3"/>
+    <hyperlink ref="H12" r:id="rId4"/>
+    <hyperlink ref="H13" r:id="rId5"/>
+    <hyperlink ref="H14" r:id="rId6"/>
+    <hyperlink ref="H15" r:id="rId7"/>
+    <hyperlink ref="H16" r:id="rId8"/>
+    <hyperlink ref="H17" r:id="rId9"/>
+    <hyperlink ref="H18" r:id="rId10"/>
+    <hyperlink ref="H19" r:id="rId11"/>
+    <hyperlink ref="H20" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
@@ -1307,22 +1446,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="6" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="7" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ eurovibes/com4bbb@8c1bc7cfa87728f9fa315841c1321edc5f412c9f 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/com4bbb-bom_0.1.xlsx
+++ b/Fabrication/BoM/com4bbb-bom_0.1.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="121">
   <si>
     <t>Row</t>
   </si>
@@ -74,6 +74,12 @@
     <t>Samsung Electro-Mechanics</t>
   </si>
   <si>
+    <t>JLCPCB</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/1877-CL05B104KO5NNNC/C1525</t>
+  </si>
+  <si>
     <t>C_0402_1005Metric</t>
   </si>
   <si>
@@ -83,76 +89,109 @@
     <t>2</t>
   </si>
   <si>
+    <t>D101 D102 D103 D104 D105 D106 D107 D108 D109 D110 D111 D112 D113</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>Hubei KENTO Elec</t>
+  </si>
+  <si>
+    <t>LED_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>Light emitting diode</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
     <t>D114</t>
   </si>
   <si>
-    <t>1N4004</t>
-  </si>
-  <si>
-    <t>D_DO-41_SOD81_P10.16mm_Horizontal</t>
-  </si>
-  <si>
-    <t>400V 1A General Purpose Rectifier Diode, DO-41</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>D101 D102 D103 D104 D105 D106 D107 D108 D109 D110 D111 D112 D113</t>
-  </si>
-  <si>
-    <t>LED</t>
-  </si>
-  <si>
-    <t>Hubei KENTO Elec</t>
-  </si>
-  <si>
-    <t>LED_0603_1608Metric</t>
-  </si>
-  <si>
-    <t>Light emitting diode</t>
-  </si>
-  <si>
-    <t>13</t>
+    <t>MRA4004T3G</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/onsemi-MRA4004T3G/C40324</t>
+  </si>
+  <si>
+    <t>D_SMA</t>
+  </si>
+  <si>
+    <t>400V, 1A, General Purpose Rectifier Diode, SMA(DO-214AC)</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
+    <t>D201</t>
+  </si>
+  <si>
+    <t>SK6812MINI</t>
+  </si>
+  <si>
+    <t>LED_SK6812MINI_PLCC4_3.5x3.5mm_P1.75mm</t>
+  </si>
+  <si>
+    <t>RGB LED with integrated controller</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>J202</t>
+  </si>
+  <si>
+    <t>Conn_01x10</t>
+  </si>
+  <si>
+    <t>JTAG</t>
+  </si>
+  <si>
+    <t>Tag-Connect_TC2050-IDC-FP_2x05_P1.27mm_Vertical</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x10, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
     <t>J101 J102</t>
   </si>
   <si>
     <t>Conn_01x02</t>
   </si>
   <si>
-    <t>PWR</t>
-  </si>
-  <si>
-    <t>TerminalBlock_Phoenix_MPT-0,5-2-2.54_1x02_P2.54mm_Horizontal</t>
+    <t>RS485</t>
+  </si>
+  <si>
+    <t>TerminalBlock_WAGO_236-402_1x02_P5.00mm_45Degree</t>
   </si>
   <si>
     <t>Generic connector, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>JP101 JP102 JP103 JP104</t>
-  </si>
-  <si>
-    <t>Jumper_3_Open</t>
-  </si>
-  <si>
-    <t>TX</t>
-  </si>
-  <si>
-    <t>SolderJumper-3_P1.3mm_Open_RoundedPad1.0x1.5mm</t>
-  </si>
-  <si>
-    <t>Jumper, 3-pole, both open</t>
-  </si>
-  <si>
-    <t>6</t>
+    <t>7</t>
+  </si>
+  <si>
+    <t>J201</t>
+  </si>
+  <si>
+    <t>USB_B_Micro</t>
+  </si>
+  <si>
+    <t>USB_Micro-B_Amphenol_10103594-0001LF_Horizontal</t>
+  </si>
+  <si>
+    <t>USB Micro Type B connector</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
   <si>
     <t>P8 P9</t>
@@ -170,7 +209,7 @@
     <t>Generic connector, double row, 02x23, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
-    <t>7</t>
+    <t>9</t>
   </si>
   <si>
     <t>R101 R102 R103 R104 R105 R106 R107 R108 R109 R110 R111 R112 R113 R114 R115 R116 R117</t>
@@ -194,7 +233,7 @@
     <t>17</t>
   </si>
   <si>
-    <t>8</t>
+    <t>10</t>
   </si>
   <si>
     <t>SW101 SW102</t>
@@ -212,61 +251,73 @@
     <t>Push button switch, normally open, two pins, 45° tilted</t>
   </si>
   <si>
-    <t>9</t>
+    <t>11</t>
+  </si>
+  <si>
+    <t>U103</t>
+  </si>
+  <si>
+    <t>AT24CS64-SSHM</t>
+  </si>
+  <si>
+    <t>AT24C512C-SSHD-T</t>
+  </si>
+  <si>
+    <t>Microchip Tech</t>
+  </si>
+  <si>
+    <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>I2C Serial EEPROM, 64Kb (8192x8) with Unique Serial Number, SO8</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>U202</t>
+  </si>
+  <si>
+    <t>ESP32-S3-WROOM-1</t>
+  </si>
+  <si>
+    <t>ESP32-S3-WROOM-1U</t>
+  </si>
+  <si>
+    <t>2.4 GHz WiFi (802.11 b/g/n) and Bluetooth ® 5 (LE) module Built around ESP32S3 series of SoCs, Xtensa ® dualcore 32bit LX7 microprocessor Flash up to 16 MB, PSRAM up to 8 MB 36 GPIOs, rich set of peripherals Onboard PCB antenna</t>
+  </si>
+  <si>
+    <t>U101</t>
+  </si>
+  <si>
+    <t>SP3485EN</t>
+  </si>
+  <si>
+    <t>MaxLinear</t>
+  </si>
+  <si>
+    <t>Industrial 3.3V Low Power Half-Duplex RS-485 Transceiver 10Mbps, SOIC-8</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>U201</t>
+  </si>
+  <si>
+    <t>USBLC6-2SC6</t>
+  </si>
+  <si>
+    <t>SOT-23-6</t>
+  </si>
+  <si>
+    <t>Very low capacitance ESD protection diode, 2 data-line, SOT-23-6</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
   <si>
     <t>U102</t>
-  </si>
-  <si>
-    <t>AT24CS64-SSHM</t>
-  </si>
-  <si>
-    <t>AT24C512C-SSHD-T</t>
-  </si>
-  <si>
-    <t>Microchip Tech</t>
-  </si>
-  <si>
-    <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>I2C Serial EEPROM, 64Kb (8192x8) with Unique Serial Number, SO8</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>U104</t>
-  </si>
-  <si>
-    <t>ESP32-WROOM-32U</t>
-  </si>
-  <si>
-    <t>Espressif Systems</t>
-  </si>
-  <si>
-    <t>RF Module, ESP32-D0WD SoC, Wi-Fi 802.11b/g/n, Bluetooth, BLE, 32-bit, 2.7-3.6V, external antenna, SMD</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>U103</t>
-  </si>
-  <si>
-    <t>SP3485EN</t>
-  </si>
-  <si>
-    <t>MaxLinear</t>
-  </si>
-  <si>
-    <t>Industrial 3.3V Low Power Half-Duplex RS-485 Transceiver 10Mbps, SOIC-8</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>U101</t>
   </si>
   <si>
     <t>WPMDH1100xx1S</t>
@@ -808,7 +859,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -825,15 +876,15 @@
     <col min="6" max="6" width="30.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
     <col min="8" max="8" width="22.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="60.7109375" customWidth="1"/>
+    <col min="9" max="9" width="60.7109375" customWidth="1"/>
+    <col min="10" max="10" width="53.7109375" customWidth="1"/>
     <col min="11" max="11" width="60.7109375" customWidth="1"/>
     <col min="12" max="12" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -847,27 +898,27 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="F2" s="3">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="F3" s="3">
         <v>46</v>
@@ -875,13 +926,13 @@
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="F4" s="3">
         <v>46</v>
@@ -889,13 +940,13 @@
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -903,13 +954,13 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="F6" s="3">
         <v>46</v>
@@ -973,232 +1024,232 @@
         <v>17</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>16</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K9" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="L9" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" ht="30" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="K12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30" customHeight="1">
+      <c r="A14" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="30" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="30" customHeight="1">
-      <c r="A12" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="K12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="45" customHeight="1">
-      <c r="A14" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H14" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="K14" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="30" customHeight="1">
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="G15" s="7" t="s">
         <v>16</v>
@@ -1216,86 +1267,86 @@
         <v>56</v>
       </c>
       <c r="L15" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="45" customHeight="1">
+      <c r="A16" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="A16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="C16" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="D16" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="E16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J16" s="9" t="s">
+      <c r="K16" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="K16" s="10" t="s">
-        <v>63</v>
-      </c>
       <c r="L16" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1">
       <c r="A17" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="C17" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="7" t="s">
+      <c r="G17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J17" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G17" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J17" s="6" t="s">
+      <c r="K17" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="K17" s="7" t="s">
+      <c r="L17" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="L17" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="30" customHeight="1">
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="8" t="s">
         <v>71</v>
       </c>
@@ -1306,13 +1357,13 @@
         <v>73</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>16</v>
@@ -1324,36 +1375,36 @@
         <v>16</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>16</v>
@@ -1362,50 +1413,164 @@
         <v>16</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="L19" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" ht="60" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="L20" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="30" customHeight="1">
+      <c r="A21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="K20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="L20" s="8" t="s">
+      <c r="K21" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="L21" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="30" customHeight="1">
+      <c r="A22" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="L22" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L23" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1426,10 +1591,13 @@
     <hyperlink ref="H18" r:id="rId10"/>
     <hyperlink ref="H19" r:id="rId11"/>
     <hyperlink ref="H20" r:id="rId12"/>
+    <hyperlink ref="H21" r:id="rId13"/>
+    <hyperlink ref="H22" r:id="rId14"/>
+    <hyperlink ref="H23" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId13"/>
+  <drawing r:id="rId16"/>
 </worksheet>
 </file>
 
@@ -1446,22 +1614,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="6" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="7" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ eurovibes/com4bbb@b88d3350758cdd2fa0de41303670df8c3ff89991 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/com4bbb-bom_0.1.xlsx
+++ b/Fabrication/BoM/com4bbb-bom_0.1.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="130">
   <si>
     <t>Row</t>
   </si>
@@ -98,6 +98,9 @@
     <t>Hubei KENTO Elec</t>
   </si>
   <si>
+    <t>https://jlcpcb.com/partdetail/Hubei_KENTOElec-KT0603R/C2286</t>
+  </si>
+  <si>
     <t>LED_0603_1608Metric</t>
   </si>
   <si>
@@ -134,6 +137,9 @@
     <t>SK6812MINI</t>
   </si>
   <si>
+    <t>https://jlcpcb.com/partdetail/OPSCOOptoelectronics-SK6812MINIHS/C2922787</t>
+  </si>
+  <si>
     <t>LED_SK6812MINI_PLCC4_3.5x3.5mm_P1.75mm</t>
   </si>
   <si>
@@ -185,6 +191,9 @@
     <t>USB_B_Micro</t>
   </si>
   <si>
+    <t>https://jlcpcb.com/partdetail/AmphenolICC-101035940001LF/C428495</t>
+  </si>
+  <si>
     <t>USB_Micro-B_Amphenol_10103594-0001LF_Horizontal</t>
   </si>
   <si>
@@ -203,6 +212,9 @@
     <t>BeagleBone_Black_Header</t>
   </si>
   <si>
+    <t>TME</t>
+  </si>
+  <si>
     <t>PinHeader_2x23_P2.54mm_Vertical</t>
   </si>
   <si>
@@ -224,6 +236,9 @@
     <t>UNI-ROYAL(Uniroyal Elec)</t>
   </si>
   <si>
+    <t>https://jlcpcb.com/partdetail/12256-0402WGF1001TCE/C11702</t>
+  </si>
+  <si>
     <t>R_0402_1005Metric</t>
   </si>
   <si>
@@ -266,6 +281,9 @@
     <t>Microchip Tech</t>
   </si>
   <si>
+    <t>https://jlcpcb.com/partdetail/MicrochipTech-AT24C256C_SSHLT/C6482</t>
+  </si>
+  <si>
     <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
   </si>
   <si>
@@ -281,6 +299,9 @@
     <t>ESP32-S3-WROOM-1</t>
   </si>
   <si>
+    <t>https://jlcpcb.com/partdetail/3522416-ESP32_S3_WROOM_1UN16R8/C3013946</t>
+  </si>
+  <si>
     <t>ESP32-S3-WROOM-1U</t>
   </si>
   <si>
@@ -296,6 +317,9 @@
     <t>MaxLinear</t>
   </si>
   <si>
+    <t>https://jlcpcb.com/partdetail/MaxLinear-SP3485EN_LTR/C8963</t>
+  </si>
+  <si>
     <t>Industrial 3.3V Low Power Half-Duplex RS-485 Transceiver 10Mbps, SOIC-8</t>
   </si>
   <si>
@@ -306,6 +330,9 @@
   </si>
   <si>
     <t>USBLC6-2SC6</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/2790619-USBLC62SC6/C2687116</t>
   </si>
   <si>
     <t>SOT-23-6</t>
@@ -884,7 +911,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -898,13 +925,13 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="F2" s="3">
         <v>15</v>
@@ -912,13 +939,13 @@
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="F3" s="3">
         <v>46</v>
@@ -926,13 +953,13 @@
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="F4" s="3">
         <v>46</v>
@@ -940,13 +967,13 @@
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -954,13 +981,13 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="F6" s="3">
         <v>46</v>
@@ -1068,30 +1095,30 @@
         <v>16</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>16</v>
@@ -1106,30 +1133,30 @@
         <v>16</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="L11" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" ht="30" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E12" s="10" t="s">
         <v>16</v>
@@ -1138,19 +1165,19 @@
         <v>16</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H12" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="L12" s="8" t="s">
         <v>12</v>
@@ -1158,16 +1185,16 @@
     </row>
     <row r="13" spans="1:12" ht="30" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>16</v>
@@ -1185,10 +1212,10 @@
         <v>16</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>12</v>
@@ -1196,16 +1223,16 @@
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>16</v>
@@ -1223,27 +1250,27 @@
         <v>16</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="L14" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>16</v>
@@ -1252,19 +1279,19 @@
         <v>16</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>16</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="L15" s="5" t="s">
         <v>12</v>
@@ -1272,16 +1299,16 @@
     </row>
     <row r="16" spans="1:12" ht="45" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>16</v>
@@ -1290,7 +1317,7 @@
         <v>16</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="H16" s="10" t="s">
         <v>16</v>
@@ -1299,10 +1326,10 @@
         <v>16</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="L16" s="8" t="s">
         <v>22</v>
@@ -1310,22 +1337,22 @@
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>18</v>
@@ -1334,30 +1361,30 @@
         <v>16</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:12">
       <c r="A18" s="8" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>16</v>
@@ -1375,10 +1402,10 @@
         <v>16</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>22</v>
@@ -1386,22 +1413,22 @@
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>18</v>
@@ -1410,13 +1437,13 @@
         <v>16</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="L19" s="5" t="s">
         <v>12</v>
@@ -1424,16 +1451,16 @@
     </row>
     <row r="20" spans="1:12" ht="60" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>16</v>
@@ -1442,19 +1469,19 @@
         <v>16</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H20" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>16</v>
+        <v>93</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>12</v>
@@ -1462,22 +1489,22 @@
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>18</v>
@@ -1486,13 +1513,13 @@
         <v>16</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>16</v>
+        <v>99</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>12</v>
@@ -1500,16 +1527,16 @@
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>16</v>
@@ -1518,19 +1545,19 @@
         <v>16</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H22" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>16</v>
+        <v>104</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>12</v>
@@ -1538,16 +1565,16 @@
     </row>
     <row r="23" spans="1:12">
       <c r="A23" s="5" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>16</v>
@@ -1565,7 +1592,7 @@
         <v>16</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>16</v>
@@ -1614,22 +1641,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="6" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="7" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ eurovibes/com4bbb@1679398a5a587527b1874f380ab776cea805480a 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/com4bbb-bom_0.1.xlsx
+++ b/Fabrication/BoM/com4bbb-bom_0.1.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="136">
   <si>
     <t>Row</t>
   </si>
@@ -158,6 +158,9 @@
     <t>JTAG</t>
   </si>
   <si>
+    <t>---</t>
+  </si>
+  <si>
     <t>Tag-Connect_TC2050-IDC-FP_2x05_P1.27mm_Vertical</t>
   </si>
   <si>
@@ -176,6 +179,12 @@
     <t>RS485</t>
   </si>
   <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>2946-236-402-ND</t>
+  </si>
+  <si>
     <t>TerminalBlock_WAGO_236-402_1x02_P5.00mm_45Degree</t>
   </si>
   <si>
@@ -215,6 +224,9 @@
     <t>TME</t>
   </si>
   <si>
+    <t>https://www.tme.eu/de/en/details/tsw-123-07-t-d/pin-headers/samtec/</t>
+  </si>
+  <si>
     <t>PinHeader_2x23_P2.54mm_Vertical</t>
   </si>
   <si>
@@ -260,6 +272,9 @@
     <t>Reset</t>
   </si>
   <si>
+    <t>https://www.tme.eu/de/en/details/tact-64n-f/microswitches-tact/ninigi/</t>
+  </si>
+  <si>
     <t>SW_PUSH_6mm</t>
   </si>
   <si>
@@ -348,6 +363,9 @@
   </si>
   <si>
     <t>WPMDH1100xx1S</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/en/details/r-78k5.0-0.5/dc-dc-converters/recom/</t>
   </si>
   <si>
     <t>KiBot Bill of Materials</t>
@@ -911,7 +929,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -925,13 +943,13 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="F2" s="3">
         <v>15</v>
@@ -939,13 +957,13 @@
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="F3" s="3">
         <v>46</v>
@@ -953,13 +971,13 @@
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="F4" s="3">
         <v>46</v>
@@ -967,13 +985,13 @@
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -981,13 +999,13 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="F6" s="3">
         <v>46</v>
@@ -1203,7 +1221,7 @@
         <v>16</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>16</v>
@@ -1212,10 +1230,10 @@
         <v>16</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>12</v>
@@ -1223,16 +1241,16 @@
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>16</v>
@@ -1241,19 +1259,19 @@
         <v>16</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>16</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="K14" s="10" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L14" s="8" t="s">
         <v>22</v>
@@ -1261,16 +1279,16 @@
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>16</v>
@@ -1285,13 +1303,13 @@
         <v>16</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="L15" s="5" t="s">
         <v>12</v>
@@ -1299,16 +1317,16 @@
     </row>
     <row r="16" spans="1:12" ht="45" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>16</v>
@@ -1317,19 +1335,19 @@
         <v>16</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="H16" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="K16" s="10" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="L16" s="8" t="s">
         <v>22</v>
@@ -1337,22 +1355,22 @@
     </row>
     <row r="17" spans="1:12" ht="30" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>18</v>
@@ -1361,30 +1379,30 @@
         <v>16</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>16</v>
@@ -1393,19 +1411,19 @@
         <v>16</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="H18" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="K18" s="10" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>22</v>
@@ -1413,22 +1431,22 @@
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>18</v>
@@ -1437,13 +1455,13 @@
         <v>16</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="K19" s="7" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="L19" s="5" t="s">
         <v>12</v>
@@ -1451,16 +1469,16 @@
     </row>
     <row r="20" spans="1:12" ht="60" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="E20" s="10" t="s">
         <v>16</v>
@@ -1475,13 +1493,13 @@
         <v>16</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="L20" s="8" t="s">
         <v>12</v>
@@ -1492,19 +1510,19 @@
         <v>29</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>18</v>
@@ -1513,13 +1531,13 @@
         <v>16</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>12</v>
@@ -1527,16 +1545,16 @@
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>16</v>
@@ -1551,30 +1569,30 @@
         <v>16</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" ht="30" customHeight="1">
       <c r="A23" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>16</v>
@@ -1583,16 +1601,16 @@
         <v>16</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>16</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>16</v>
+        <v>115</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>16</v>
@@ -1641,22 +1659,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="6" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="7" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ eurovibes/com4bbb@4d958de001089e8659ce9f94b155ed1b126b3772 🚀
</commit_message>
<xml_diff>
--- a/Fabrication/BoM/com4bbb-bom_0.1.xlsx
+++ b/Fabrication/BoM/com4bbb-bom_0.1.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="160">
   <si>
     <t>Row</t>
   </si>
@@ -59,7 +59,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>C101</t>
+    <t>C101 C102</t>
   </si>
   <si>
     <t>C</t>
@@ -89,6 +89,48 @@
     <t>2</t>
   </si>
   <si>
+    <t>C103 C104</t>
+  </si>
+  <si>
+    <t>C_Polarized</t>
+  </si>
+  <si>
+    <t>1 F</t>
+  </si>
+  <si>
+    <t>TME</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/en/details/scv1f-3.0v-ltz/supercapacitors/spscap/scv0001c0-003r0ltz/</t>
+  </si>
+  <si>
+    <t>CP_Radial_D8.0mm_P3.50mm</t>
+  </si>
+  <si>
+    <t>Polarized capacitor</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>D115</t>
+  </si>
+  <si>
+    <t>1N5819WS</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/GuangdongHottech-1N5819WS/C191023</t>
+  </si>
+  <si>
+    <t>D_SOD-323</t>
+  </si>
+  <si>
+    <t>40V 600mV@1A 1A SOD-323 Schottky Barrier Diodes, SOD-323</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
     <t>D101 D102 D103 D104 D105 D106 D107 D108 D109 D110 D111 D112 D113</t>
   </si>
   <si>
@@ -110,7 +152,7 @@
     <t>13</t>
   </si>
   <si>
-    <t>3</t>
+    <t>5</t>
   </si>
   <si>
     <t>D114</t>
@@ -128,7 +170,7 @@
     <t>400V, 1A, General Purpose Rectifier Diode, SMA(DO-214AC)</t>
   </si>
   <si>
-    <t>4</t>
+    <t>6</t>
   </si>
   <si>
     <t>D201</t>
@@ -146,7 +188,7 @@
     <t>RGB LED with integrated controller</t>
   </si>
   <si>
-    <t>5</t>
+    <t>7</t>
   </si>
   <si>
     <t>J202</t>
@@ -167,7 +209,7 @@
     <t>Generic connector, single row, 01x10, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
-    <t>6</t>
+    <t>8</t>
   </si>
   <si>
     <t>J101 J102</t>
@@ -191,7 +233,7 @@
     <t>Generic connector, single row, 01x02, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
-    <t>7</t>
+    <t>9</t>
   </si>
   <si>
     <t>J201</t>
@@ -209,7 +251,7 @@
     <t>USB Micro Type B connector</t>
   </si>
   <si>
-    <t>8</t>
+    <t>10</t>
   </si>
   <si>
     <t>P8 P9</t>
@@ -221,9 +263,6 @@
     <t>BeagleBone_Black_Header</t>
   </si>
   <si>
-    <t>TME</t>
-  </si>
-  <si>
     <t>https://www.tme.eu/de/en/details/tsw-123-07-t-d/pin-headers/samtec/</t>
   </si>
   <si>
@@ -233,10 +272,10 @@
     <t>Generic connector, double row, 02x23, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>R101 R102 R103 R104 R105 R106 R107 R108 R109 R110 R111 R112 R113 R114 R115 R116 R117</t>
+    <t>11</t>
+  </si>
+  <si>
+    <t>R101 R102 R103 R104 R105 R106 R107 R108 R109 R110 R111 R112 R113 R114 R115 R116 R117 R118</t>
   </si>
   <si>
     <t>R</t>
@@ -248,7 +287,7 @@
     <t>UNI-ROYAL(Uniroyal Elec)</t>
   </si>
   <si>
-    <t>https://jlcpcb.com/partdetail/12256-0402WGF1001TCE/C11702</t>
+    <t>https://jlcpcb.com/partdetail/12256-0402WGF1001TCE/C11702 https://jlcpcb.com/partdetail/18168-0805W8F150JT5E/C17480</t>
   </si>
   <si>
     <t>R_0402_1005Metric</t>
@@ -257,70 +296,115 @@
     <t>Resistor</t>
   </si>
   <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>SW101 SW102</t>
+  </si>
+  <si>
+    <t>SW_Push_45deg</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/en/details/tact-64n-f/microswitches-tact/ninigi/</t>
+  </si>
+  <si>
+    <t>SW_PUSH_6mm</t>
+  </si>
+  <si>
+    <t>Push button switch, normally open, two pins, 45° tilted</t>
+  </si>
+  <si>
+    <t>U103</t>
+  </si>
+  <si>
+    <t>AT24CS64-SSHM</t>
+  </si>
+  <si>
+    <t>AT24C512C-SSHD-T</t>
+  </si>
+  <si>
+    <t>Microchip Tech</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/MicrochipTech-AT24C256C_SSHLT/C6482</t>
+  </si>
+  <si>
+    <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
+  </si>
+  <si>
+    <t>I2C Serial EEPROM, 64Kb (8192x8) with Unique Serial Number, SO8</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>U104</t>
+  </si>
+  <si>
+    <t>ATECC608A-MAHDA</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/MicrochipTech-ATECC608B_MAHDAT/C17561150</t>
+  </si>
+  <si>
+    <t>DFN-8-1EP_3x2mm_P0.5mm_EP1.3x1.5mm</t>
+  </si>
+  <si>
+    <t>Cryptographic Co-Processor with Secure Hardware-based 16 Key Storage, ECDSA and ECDH support, I2C, UDFN-8</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>U105</t>
+  </si>
+  <si>
+    <t>DS3231MZ</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/108629-DS3231MZTRL/C107410</t>
+  </si>
+  <si>
+    <t>±5ppm, I2C Real-Time Clock SOIC-8</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>U202</t>
+  </si>
+  <si>
+    <t>ESP32-S3-WROOM-1</t>
+  </si>
+  <si>
+    <t>https://jlcpcb.com/partdetail/3522416-ESP32_S3_WROOM_1UN16R8/C3013946</t>
+  </si>
+  <si>
+    <t>ESP32-S3-WROOM-1U</t>
+  </si>
+  <si>
+    <t>2.4 GHz WiFi (802.11 b/g/n) and Bluetooth ® 5 (LE) module Built around ESP32S3 series of SoCs, Xtensa ® dualcore 32bit LX7 microprocessor Flash up to 16 MB, PSRAM up to 8 MB 36 GPIOs, rich set of peripherals Onboard PCB antenna</t>
+  </si>
+  <si>
     <t>17</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>SW101 SW102</t>
-  </si>
-  <si>
-    <t>SW_Push_45deg</t>
-  </si>
-  <si>
-    <t>Reset</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/de/en/details/tact-64n-f/microswitches-tact/ninigi/</t>
-  </si>
-  <si>
-    <t>SW_PUSH_6mm</t>
-  </si>
-  <si>
-    <t>Push button switch, normally open, two pins, 45° tilted</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>U103</t>
-  </si>
-  <si>
-    <t>AT24CS64-SSHM</t>
-  </si>
-  <si>
-    <t>AT24C512C-SSHD-T</t>
-  </si>
-  <si>
-    <t>Microchip Tech</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/MicrochipTech-AT24C256C_SSHLT/C6482</t>
-  </si>
-  <si>
-    <t>SOIC-8_3.9x4.9mm_P1.27mm</t>
-  </si>
-  <si>
-    <t>I2C Serial EEPROM, 64Kb (8192x8) with Unique Serial Number, SO8</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>U202</t>
-  </si>
-  <si>
-    <t>ESP32-S3-WROOM-1</t>
-  </si>
-  <si>
-    <t>https://jlcpcb.com/partdetail/3522416-ESP32_S3_WROOM_1UN16R8/C3013946</t>
-  </si>
-  <si>
-    <t>ESP32-S3-WROOM-1U</t>
-  </si>
-  <si>
-    <t>2.4 GHz WiFi (802.11 b/g/n) and Bluetooth ® 5 (LE) module Built around ESP32S3 series of SoCs, Xtensa ® dualcore 32bit LX7 microprocessor Flash up to 16 MB, PSRAM up to 8 MB 36 GPIOs, rich set of peripherals Onboard PCB antenna</t>
+    <t>U102</t>
+  </si>
+  <si>
+    <t>WPMDH1100xx1S</t>
+  </si>
+  <si>
+    <t>R-78K5.0-0.5</t>
+  </si>
+  <si>
+    <t>https://www.tme.eu/de/en/details/r-78k5.0-0.5/dc-dc-converters/recom/</t>
   </si>
   <si>
     <t>U101</t>
@@ -338,7 +422,7 @@
     <t>Industrial 3.3V Low Power Half-Duplex RS-485 Transceiver 10Mbps, SOIC-8</t>
   </si>
   <si>
-    <t>14</t>
+    <t>19</t>
   </si>
   <si>
     <t>U201</t>
@@ -354,18 +438,6 @@
   </si>
   <si>
     <t>Very low capacitance ESD protection diode, 2 data-line, SOT-23-6</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>U102</t>
-  </si>
-  <si>
-    <t>WPMDH1100xx1S</t>
-  </si>
-  <si>
-    <t>https://www.tme.eu/de/en/details/r-78k5.0-0.5/dc-dc-converters/recom/</t>
   </si>
   <si>
     <t>KiBot Bill of Materials</t>
@@ -904,7 +976,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
@@ -929,7 +1001,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="32" customHeight="1">
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>140</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -943,55 +1015,55 @@
     </row>
     <row r="2" spans="1:12">
       <c r="C2" s="2" t="s">
-        <v>117</v>
+        <v>141</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="F2" s="3">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="C3" s="2" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>120</v>
+        <v>144</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="F3" s="3">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="C4" s="2" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="F4" s="3">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="C5" s="2" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="F5" s="3">
         <v>1</v>
@@ -999,16 +1071,16 @@
     </row>
     <row r="6" spans="1:12">
       <c r="C6" s="2" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="F6" s="3">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1084,7 +1156,7 @@
         <v>21</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1">
@@ -1098,34 +1170,34 @@
         <v>24</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>16</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>16</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -1180,7 +1252,7 @@
         <v>16</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>18</v>
@@ -1189,30 +1261,30 @@
         <v>16</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="30" customHeight="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>16</v>
@@ -1221,19 +1293,19 @@
         <v>16</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>16</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L13" s="5" t="s">
         <v>12</v>
@@ -1241,13 +1313,13 @@
     </row>
     <row r="14" spans="1:12" ht="30" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>52</v>
@@ -1259,33 +1331,33 @@
         <v>16</v>
       </c>
       <c r="G14" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="J14" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="I14" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J14" s="9" t="s">
+      <c r="K14" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="K14" s="10" t="s">
-        <v>56</v>
-      </c>
       <c r="L14" s="8" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30" customHeight="1">
       <c r="A15" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>59</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>59</v>
@@ -1297,13 +1369,13 @@
         <v>16</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>16</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>61</v>
@@ -1315,7 +1387,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="45" customHeight="1">
+    <row r="16" spans="1:12" ht="30" customHeight="1">
       <c r="A16" s="8" t="s">
         <v>63</v>
       </c>
@@ -1338,10 +1410,10 @@
         <v>67</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>69</v>
@@ -1364,13 +1436,13 @@
         <v>73</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>16</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>75</v>
+        <v>16</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>18</v>
@@ -1379,51 +1451,51 @@
         <v>16</v>
       </c>
       <c r="I17" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="K17" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="L17" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="45" customHeight="1">
+      <c r="A18" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="K17" s="7" t="s">
+      <c r="B18" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="C18" s="9" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="30" customHeight="1">
-      <c r="A18" s="8" t="s">
+      <c r="D18" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="E18" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="J18" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="K18" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="H18" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="J18" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="K18" s="10" t="s">
-        <v>86</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>22</v>
@@ -1431,22 +1503,22 @@
     </row>
     <row r="19" spans="1:12" ht="30" customHeight="1">
       <c r="A19" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="E19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>88</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>91</v>
       </c>
       <c r="G19" s="7" t="s">
         <v>18</v>
@@ -1455,65 +1527,65 @@
         <v>16</v>
       </c>
       <c r="I19" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="L19" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="J19" s="6" t="s">
+    </row>
+    <row r="20" spans="1:12" ht="30" customHeight="1">
+      <c r="A20" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="K19" s="7" t="s">
+      <c r="B20" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="L19" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="60" customHeight="1">
-      <c r="A20" s="8" t="s">
+      <c r="C20" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="D20" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="E20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="10" t="s">
+      <c r="J20" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="J20" s="9" t="s">
+      <c r="K20" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="K20" s="10" t="s">
-        <v>100</v>
-      </c>
       <c r="L20" s="8" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="30" customHeight="1">
       <c r="A21" s="5" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>102</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>102</v>
@@ -1534,10 +1606,10 @@
         <v>104</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="L21" s="5" t="s">
         <v>12</v>
@@ -1545,16 +1617,16 @@
     </row>
     <row r="22" spans="1:12" ht="30" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>16</v>
@@ -1569,30 +1641,30 @@
         <v>16</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K22" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="L22" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="30" customHeight="1">
+    <row r="23" spans="1:12">
       <c r="A23" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>16</v>
@@ -1601,21 +1673,173 @@
         <v>16</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>16</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="L23" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="60" customHeight="1">
+      <c r="A24" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="K24" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="L24" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="30" customHeight="1">
+      <c r="A25" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L25" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="30" customHeight="1">
+      <c r="A26" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="K26" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="L26" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="30" customHeight="1">
+      <c r="A27" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="L27" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1639,10 +1863,14 @@
     <hyperlink ref="H21" r:id="rId13"/>
     <hyperlink ref="H22" r:id="rId14"/>
     <hyperlink ref="H23" r:id="rId15"/>
+    <hyperlink ref="H24" r:id="rId16"/>
+    <hyperlink ref="H25" r:id="rId17"/>
+    <hyperlink ref="H26" r:id="rId18"/>
+    <hyperlink ref="H27" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId16"/>
+  <drawing r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -1659,22 +1887,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="6" t="s">
-        <v>133</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>134</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="7" t="s">
-        <v>135</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>